<commit_message>
intento de correjir columna de Art
</commit_message>
<xml_diff>
--- a/promedios ivan modificados.xlsx
+++ b/promedios ivan modificados.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="548">
   <si>
     <t xml:space="preserve">NOMBRE</t>
   </si>
@@ -327,6 +327,9 @@
     <t xml:space="preserve">Balance45!</t>
   </si>
   <si>
+    <t xml:space="preserve">Art Album</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prom. estimado enero</t>
   </si>
   <si>
@@ -594,9 +597,6 @@
     <t xml:space="preserve">Concerns44#</t>
   </si>
   <si>
-    <t xml:space="preserve">Art Album..</t>
-  </si>
-  <si>
     <t xml:space="preserve">ACOSTA LOPEZ LUNA SOPHIA</t>
   </si>
   <si>
@@ -1140,9 +1140,6 @@
     <t xml:space="preserve">Fortress45(</t>
   </si>
   <si>
-    <t xml:space="preserve">Art album.</t>
-  </si>
-  <si>
     <t xml:space="preserve">ACEVEDO RAMIREZ ANGEL GIBRAN</t>
   </si>
   <si>
@@ -1405,9 +1402,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jubilant44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Art album..</t>
   </si>
   <si>
     <t xml:space="preserve">AGUILAR MARQUEZ JOSE GABRIEL</t>
@@ -1681,11 +1675,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -2213,7 +2206,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2453,11 +2446,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2752,8 +2745,8 @@
   </sheetPr>
   <dimension ref="A1:AC46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5435,7 +5428,7 @@
       <c r="AB44" s="29"/>
       <c r="AC44" s="29"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="n">
         <v>44</v>
       </c>
@@ -5496,7 +5489,7 @@
       <c r="AB45" s="29"/>
       <c r="AC45" s="29"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="n">
         <v>45</v>
       </c>
@@ -5559,7 +5552,7 @@
   <dimension ref="A1:AC46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5567,7 +5560,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -5579,7 +5572,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -5599,7 +5592,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="10"/>
@@ -5623,10 +5616,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" s="70" t="n">
         <f aca="false">5+5</f>
@@ -5684,10 +5677,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3" s="70" t="n">
         <f aca="false">4+5</f>
@@ -5745,10 +5738,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D4" s="70" t="n">
         <f aca="false">5+5</f>
@@ -5806,10 +5799,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="70" t="n">
         <f aca="false">4.5+5</f>
@@ -5867,10 +5860,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" s="70" t="n">
         <f aca="false">5+5</f>
@@ -5928,10 +5921,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="70" t="n">
         <f aca="false">5+5</f>
@@ -5989,10 +5982,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D8" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6050,10 +6043,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" s="70" t="n">
         <f aca="false">3+5</f>
@@ -6111,10 +6104,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6172,10 +6165,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D11" s="70" t="n">
         <f aca="false">3+5</f>
@@ -6233,10 +6226,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D12" s="70" t="n">
         <f aca="false">0+5</f>
@@ -6294,10 +6287,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D13" s="70" t="n">
         <f aca="false">4+5</f>
@@ -6355,10 +6348,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D14" s="70" t="n">
         <f aca="false">3.5+5</f>
@@ -6416,10 +6409,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D15" s="70" t="n">
         <f aca="false">4+5</f>
@@ -6477,10 +6470,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D16" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6538,10 +6531,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D17" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6599,10 +6592,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D18" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6660,10 +6653,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D19" s="70" t="n">
         <f aca="false">3+5</f>
@@ -6721,10 +6714,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D20" s="70" t="n">
         <f aca="false">2.5+4</f>
@@ -6782,10 +6775,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D21" s="70" t="n">
         <f aca="false">1.5+5</f>
@@ -6843,10 +6836,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D22" s="70" t="n">
         <f aca="false">3.5+5</f>
@@ -6904,10 +6897,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D23" s="70" t="n">
         <f aca="false">5+5</f>
@@ -6965,10 +6958,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D24" s="70" t="n">
         <f aca="false">1.5+4</f>
@@ -7026,10 +7019,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D25" s="70" t="n">
         <f aca="false">2.5+4</f>
@@ -7087,10 +7080,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" s="70" t="n">
         <f aca="false">2+4</f>
@@ -7148,10 +7141,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D27" s="70" t="n">
         <f aca="false">3+5</f>
@@ -7209,10 +7202,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D28" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7270,10 +7263,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D29" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7331,10 +7324,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D30" s="70" t="n">
         <f aca="false">1.5+4</f>
@@ -7392,10 +7385,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D31" s="70" t="n">
         <f aca="false">2+4</f>
@@ -7453,10 +7446,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D32" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7514,10 +7507,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D33" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7575,10 +7568,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D34" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7636,10 +7629,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D35" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7697,10 +7690,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7758,10 +7751,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D37" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7819,10 +7812,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D38" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7880,10 +7873,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D39" s="70" t="n">
         <f aca="false">0+5</f>
@@ -7936,15 +7929,15 @@
       <c r="AB39" s="37"/>
       <c r="AC39" s="38"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="27" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D40" s="70" t="n">
         <f aca="false">5+5</f>
@@ -7997,15 +7990,15 @@
       <c r="AB40" s="47"/>
       <c r="AC40" s="48"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D41" s="70" t="n">
         <f aca="false">5+5</f>
@@ -8058,15 +8051,15 @@
       <c r="AB41" s="59"/>
       <c r="AC41" s="13"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D42" s="70" t="n">
         <f aca="false">5+5</f>
@@ -8119,15 +8112,15 @@
       <c r="AB42" s="37"/>
       <c r="AC42" s="38"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D43" s="70" t="n">
         <f aca="false">1+4</f>
@@ -8178,15 +8171,15 @@
       <c r="AB43" s="37"/>
       <c r="AC43" s="38"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D44" s="70" t="n">
         <f aca="false">5+5</f>
@@ -8239,15 +8232,15 @@
       <c r="AB44" s="29"/>
       <c r="AC44" s="29"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="n">
         <v>44</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D45" s="70" t="n">
         <f aca="false">5+5</f>
@@ -8319,8 +8312,8 @@
   </sheetPr>
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8328,7 +8321,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -8340,7 +8333,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -8360,7 +8353,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="94"/>
       <c r="O1" s="97"/>
@@ -9594,7 +9587,7 @@
       <c r="AB21" s="37"/>
       <c r="AC21" s="38"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="n">
         <v>21</v>
       </c>
@@ -9655,7 +9648,7 @@
       <c r="AB22" s="47"/>
       <c r="AC22" s="48"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="n">
         <v>22</v>
       </c>
@@ -9716,7 +9709,7 @@
       <c r="AB23" s="59"/>
       <c r="AC23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="n">
         <v>23</v>
       </c>
@@ -9777,7 +9770,7 @@
       <c r="AB24" s="26"/>
       <c r="AC24" s="23"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="n">
         <v>24</v>
       </c>
@@ -9838,7 +9831,7 @@
       <c r="AB25" s="37"/>
       <c r="AC25" s="38"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="n">
         <v>25</v>
       </c>
@@ -9899,7 +9892,7 @@
       <c r="AB26" s="37"/>
       <c r="AC26" s="38"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="n">
         <v>26</v>
       </c>
@@ -9960,7 +9953,7 @@
       <c r="AB27" s="37"/>
       <c r="AC27" s="38"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="n">
         <v>27</v>
       </c>
@@ -10997,7 +10990,7 @@
       <c r="AB44" s="37"/>
       <c r="AC44" s="38"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="n">
         <v>44</v>
       </c>
@@ -11058,7 +11051,7 @@
       <c r="AB45" s="47"/>
       <c r="AC45" s="48"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="n">
         <v>45</v>
       </c>
@@ -11166,7 +11159,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -11198,7 +11191,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="94"/>
       <c r="O1" s="97"/>
@@ -13986,7 +13979,7 @@
   <dimension ref="A1:AC45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13994,7 +13987,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -14006,7 +13999,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>371</v>
+        <v>281</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -14026,7 +14019,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="94"/>
       <c r="O1" s="97"/>
@@ -14050,10 +14043,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>372</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>373</v>
       </c>
       <c r="D2" s="36" t="n">
         <f aca="false">0+5</f>
@@ -14111,10 +14104,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>374</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>375</v>
       </c>
       <c r="D3" s="36" t="n">
         <f aca="false">0+4</f>
@@ -14172,10 +14165,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>376</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>377</v>
       </c>
       <c r="D4" s="36" t="n">
         <f aca="false">2+3</f>
@@ -14233,10 +14226,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>378</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>379</v>
       </c>
       <c r="D5" s="36" t="n">
         <f aca="false">5+4.5</f>
@@ -14294,10 +14287,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>380</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>381</v>
       </c>
       <c r="D6" s="36" t="n">
         <f aca="false">2+4</f>
@@ -14355,10 +14348,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>382</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>383</v>
       </c>
       <c r="D7" s="36" t="n">
         <f aca="false">5+5</f>
@@ -14416,10 +14409,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>384</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>385</v>
       </c>
       <c r="D8" s="36" t="n">
         <f aca="false">5+2</f>
@@ -14477,10 +14470,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>386</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>387</v>
       </c>
       <c r="D9" s="36" t="n">
         <f aca="false">5+5</f>
@@ -14538,10 +14531,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="38" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>388</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>389</v>
       </c>
       <c r="D10" s="36" t="n">
         <f aca="false">4.5+4</f>
@@ -14599,10 +14592,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>390</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>391</v>
       </c>
       <c r="D11" s="36" t="n">
         <f aca="false">4+1</f>
@@ -14660,10 +14653,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="C12" s="38" t="s">
         <v>392</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>393</v>
       </c>
       <c r="D12" s="36" t="n">
         <f aca="false">5+5</f>
@@ -14721,10 +14714,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>394</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>395</v>
       </c>
       <c r="D13" s="36" t="n">
         <f aca="false">3+5</f>
@@ -14782,10 +14775,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>396</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>397</v>
       </c>
       <c r="D14" s="36" t="n">
         <f aca="false">5+4</f>
@@ -14843,10 +14836,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>398</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>399</v>
       </c>
       <c r="D15" s="36" t="n">
         <f aca="false">2+5</f>
@@ -14904,10 +14897,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>400</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>401</v>
       </c>
       <c r="D16" s="36" t="n">
         <f aca="false">3+2</f>
@@ -14965,10 +14958,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>402</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>403</v>
       </c>
       <c r="D17" s="36" t="n">
         <f aca="false">5+5</f>
@@ -15026,10 +15019,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>404</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>405</v>
       </c>
       <c r="D18" s="36" t="n">
         <f aca="false">5+5</f>
@@ -15087,10 +15080,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>406</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>407</v>
       </c>
       <c r="D19" s="36" t="n">
         <f aca="false">1.5+5</f>
@@ -15148,10 +15141,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>408</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>409</v>
       </c>
       <c r="D20" s="36" t="n">
         <f aca="false">4+5</f>
@@ -15209,10 +15202,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C21" s="38" t="s">
         <v>410</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>411</v>
       </c>
       <c r="D21" s="36" t="n">
         <f aca="false">4+5</f>
@@ -15270,10 +15263,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="113" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22" s="113" t="s">
         <v>412</v>
-      </c>
-      <c r="C22" s="113" t="s">
-        <v>413</v>
       </c>
       <c r="D22" s="36" t="n">
         <f aca="false">1+4</f>
@@ -15331,10 +15324,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="C23" s="38" t="s">
         <v>414</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>415</v>
       </c>
       <c r="D23" s="36" t="n">
         <f aca="false">4+5</f>
@@ -15392,10 +15385,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" s="38" t="s">
         <v>416</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>417</v>
       </c>
       <c r="D24" s="36" t="n">
         <f aca="false">5+3</f>
@@ -15453,10 +15446,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="C25" s="38" t="s">
         <v>418</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>419</v>
       </c>
       <c r="D25" s="36" t="n">
         <f aca="false">5+5</f>
@@ -15514,10 +15507,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="C26" s="38" t="s">
         <v>420</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>421</v>
       </c>
       <c r="D26" s="36" t="n">
         <f aca="false">4+5</f>
@@ -15575,10 +15568,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>422</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>423</v>
       </c>
       <c r="D27" s="36" t="n">
         <f aca="false">2.5+5</f>
@@ -15634,10 +15627,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="C28" s="38" t="s">
         <v>424</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>425</v>
       </c>
       <c r="D28" s="36" t="n">
         <f aca="false">3.5+4</f>
@@ -15695,10 +15688,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="C29" s="38" t="s">
         <v>426</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>427</v>
       </c>
       <c r="D29" s="36" t="n">
         <f aca="false">4+5</f>
@@ -15756,10 +15749,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="38" t="s">
         <v>428</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>429</v>
       </c>
       <c r="D30" s="36" t="n">
         <f aca="false">5+5</f>
@@ -15817,10 +15810,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="C31" s="38" t="s">
         <v>430</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>431</v>
       </c>
       <c r="D31" s="36" t="n">
         <f aca="false">4+4</f>
@@ -15878,10 +15871,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="38" t="s">
+        <v>431</v>
+      </c>
+      <c r="C32" s="38" t="s">
         <v>432</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>433</v>
       </c>
       <c r="D32" s="36" t="n">
         <f aca="false">2.5+5</f>
@@ -15939,10 +15932,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>434</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>435</v>
       </c>
       <c r="D33" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16000,10 +15993,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="C34" s="38" t="s">
         <v>436</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>437</v>
       </c>
       <c r="D34" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16061,10 +16054,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="38" t="s">
+        <v>437</v>
+      </c>
+      <c r="C35" s="38" t="s">
         <v>438</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>439</v>
       </c>
       <c r="D35" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16122,10 +16115,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="38" t="s">
+        <v>439</v>
+      </c>
+      <c r="C36" s="38" t="s">
         <v>440</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>441</v>
       </c>
       <c r="D36" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16183,10 +16176,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>442</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>443</v>
       </c>
       <c r="D37" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16244,10 +16237,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="C38" s="38" t="s">
         <v>444</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>445</v>
       </c>
       <c r="D38" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16305,10 +16298,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C39" s="38" t="s">
         <v>446</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>447</v>
       </c>
       <c r="D39" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16366,10 +16359,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="38" t="s">
+        <v>447</v>
+      </c>
+      <c r="C40" s="38" t="s">
         <v>448</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>449</v>
       </c>
       <c r="D40" s="36" t="n">
         <f aca="false">4+5</f>
@@ -16427,10 +16420,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="C41" s="38" t="s">
         <v>450</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>451</v>
       </c>
       <c r="D41" s="36" t="n">
         <f aca="false">1.5+5</f>
@@ -16488,10 +16481,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="38" t="s">
+        <v>451</v>
+      </c>
+      <c r="C42" s="38" t="s">
         <v>452</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>453</v>
       </c>
       <c r="D42" s="36" t="n">
         <f aca="false">5+5</f>
@@ -16549,10 +16542,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="38" t="s">
+        <v>453</v>
+      </c>
+      <c r="C43" s="38" t="s">
         <v>454</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>455</v>
       </c>
       <c r="D43" s="36" t="n">
         <f aca="false">4.5+5</f>
@@ -16610,10 +16603,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>456</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>457</v>
       </c>
       <c r="D44" s="120" t="n">
         <f aca="false">1+1</f>
@@ -16654,10 +16647,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="133" t="s">
+        <v>457</v>
+      </c>
+      <c r="C45" s="133" t="s">
         <v>458</v>
-      </c>
-      <c r="C45" s="133" t="s">
-        <v>459</v>
       </c>
       <c r="D45" s="120" t="n">
         <v>10</v>
@@ -16710,8 +16703,8 @@
   </sheetPr>
   <dimension ref="A1:AC46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16719,7 +16712,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -16731,7 +16724,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -16751,7 +16744,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="94"/>
       <c r="O1" s="97"/>
@@ -16775,10 +16768,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D2" s="135" t="n">
         <f aca="false">2.5+4</f>
@@ -16836,10 +16829,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D3" s="135" t="n">
         <f aca="false">4+5</f>
@@ -16897,10 +16890,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D4" s="135" t="n">
         <f aca="false">4.5+5</f>
@@ -16958,10 +16951,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D5" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17019,10 +17012,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D6" s="135" t="n">
         <f aca="false">0+5</f>
@@ -17080,10 +17073,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D7" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17141,10 +17134,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D8" s="135" t="n">
         <f aca="false">5+4</f>
@@ -17202,10 +17195,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D9" s="135" t="n">
         <f aca="false">4+5</f>
@@ -17263,10 +17256,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D10" s="135" t="n">
         <f aca="false">4+5</f>
@@ -17324,10 +17317,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D11" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17385,10 +17378,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D12" s="135" t="n">
         <f aca="false">2+5</f>
@@ -17446,10 +17439,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D13" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17507,10 +17500,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D14" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17568,10 +17561,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D15" s="135" t="n">
         <f aca="false">0+5</f>
@@ -17629,10 +17622,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D16" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17690,10 +17683,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D17" s="135" t="n">
         <f aca="false">5+5</f>
@@ -17751,10 +17744,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D18" s="135" t="n">
         <f aca="false">1.5+5</f>
@@ -17812,10 +17805,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D19" s="135" t="n">
         <f aca="false">3.5+5</f>
@@ -17873,10 +17866,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D20" s="135" t="n">
         <f aca="false">1+5</f>
@@ -17934,10 +17927,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D21" s="135" t="n">
         <f aca="false">0+5</f>
@@ -17995,10 +17988,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D22" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18056,10 +18049,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D23" s="135" t="n">
         <f aca="false">3+5</f>
@@ -18117,10 +18110,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D24" s="135" t="n">
         <f aca="false">2+5</f>
@@ -18178,10 +18171,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D25" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18239,10 +18232,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D26" s="135" t="n">
         <f aca="false">0+5</f>
@@ -18300,10 +18293,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D27" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18361,10 +18354,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D28" s="135" t="n">
         <f aca="false">4+5</f>
@@ -18422,10 +18415,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D29" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18483,10 +18476,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D30" s="135" t="n">
         <f aca="false">0+5</f>
@@ -18544,10 +18537,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D31" s="135" t="n">
         <f aca="false">5+4</f>
@@ -18605,10 +18598,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D32" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18666,10 +18659,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D33" s="135" t="n">
         <f aca="false">1.5+5</f>
@@ -18727,10 +18720,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D34" s="135" t="n">
         <f aca="false">5+5</f>
@@ -18788,10 +18781,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D35" s="135" t="n">
         <f aca="false">1+5</f>
@@ -18849,10 +18842,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D36" s="135" t="n">
         <f aca="false">1.5+4</f>
@@ -18910,10 +18903,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D37" s="135" t="n">
         <f aca="false">2+4</f>
@@ -18971,10 +18964,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D38" s="135" t="n">
         <f aca="false">3.5+5</f>
@@ -19032,10 +19025,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D39" s="135" t="n">
         <f aca="false">5+4</f>
@@ -19093,10 +19086,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D40" s="135" t="n">
         <f aca="false">3+5</f>
@@ -19154,10 +19147,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D41" s="135" t="n">
         <f aca="false">4.5+5</f>
@@ -19215,10 +19208,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D42" s="135" t="n">
         <f aca="false">3+5</f>
@@ -19276,10 +19269,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D43" s="135" t="n">
         <f aca="false">3.5+5</f>
@@ -19337,10 +19330,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D44" s="135" t="n">
         <f aca="false">4.5+4</f>
@@ -19398,10 +19391,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D45" s="36"/>
       <c r="E45" s="6" t="n">
@@ -19440,7 +19433,7 @@
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="48" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="46"/>

</xml_diff>